<commit_message>
creacion carpeta generarScriptJS y archivos
</commit_message>
<xml_diff>
--- a/Ejercicios_Python/herramientasBasicas/pasajeros.xlsx
+++ b/Ejercicios_Python/herramientasBasicas/pasajeros.xlsx
@@ -18,7 +18,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -30,14 +30,6 @@
       <name val="Calibri"/>
       <color theme="1"/>
       <sz val="10"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <color theme="1"/>
-      <sz val="10"/>
-      <u val="single"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -61,11 +53,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -412,7 +403,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -1030,7 +1021,7 @@
           <t>autos</t>
         </is>
       </c>
-      <c r="B15" s="3" t="n">
+      <c r="B15" s="1" t="n">
         <v>1</v>
       </c>
       <c r="C15" s="1" t="n">

</xml_diff>